<commit_message>
Add an empty sheet
</commit_message>
<xml_diff>
--- a/foo.xlsx
+++ b/foo.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="money-in" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="money-out" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="empty-sheet" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -64,6 +65,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -228,7 +230,7 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -284,7 +286,33 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>

<commit_message>
Access data from individual cells
</commit_message>
<xml_diff>
--- a/foo.xlsx
+++ b/foo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="money-in" sheetId="1" state="visible" r:id="rId2"/>
@@ -55,10 +55,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-C0A];[RED]\-#,##0.00\ [$€-C0A]"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -125,7 +126,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -135,6 +136,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -157,8 +162,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -231,7 +236,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="A2:A4 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -251,7 +256,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="3" t="n">
         <v>43921</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -262,7 +267,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="3" t="n">
         <v>43918</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -273,7 +278,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="3" t="n">
         <v>43879</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -301,8 +306,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>